<commit_message>
Correcciones Cobranzas por prestaciones e incorporacion del campo Origen
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Cobranza por Prestaciones/Grupo Prestaciones.xlsx
+++ b/DBA/Reportes BI/2021/Cobranza por Prestaciones/Grupo Prestaciones.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personales\Sistemas\Agustin\Reportes BI\2021\Facturación\Automatizado\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Cobranza por Prestaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="367">
   <si>
     <t>Prestacion</t>
   </si>
@@ -1122,12 +1122,15 @@
   </si>
   <si>
     <t>25.05</t>
+  </si>
+  <si>
+    <t>IAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1256,8 +1259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B358" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B358"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B359" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B359"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Prestacion" dataDxfId="1"/>
     <tableColumn id="2" name="Grupo de Prestaciones" dataDxfId="0"/>
@@ -1529,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B358"/>
+  <dimension ref="A1:B359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="A357" sqref="A357"/>
+    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
+      <selection activeCell="B366" sqref="B366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4405,6 +4408,14 @@
         <v>318</v>
       </c>
     </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>